<commit_message>
https://leetcode.com/problems/coin-change/ Made it to the same backtrack combo
</commit_message>
<xml_diff>
--- a/codingHelper.xlsx
+++ b/codingHelper.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kumeshba/coding/algorithmsAndDataStrucures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC556699-ED27-3348-953F-ABEA62B2A877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385513E3-27DE-454B-9AE5-D2A1A43842E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20480" yWindow="500" windowWidth="20480" windowHeight="22540" xr2:uid="{E5EEE7EB-6BCC-844F-B773-BEAE663F02A3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="16300" activeTab="1" xr2:uid="{E5EEE7EB-6BCC-844F-B773-BEAE663F02A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="backtrack shortcut" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -237,6 +238,63 @@
   </si>
   <si>
     <t>Alice needs to get more chances to remove than Bob because Alice goes first. Therefore, even if they have equal chances and Alice goes first, Bob wins, since Bob had more chances than Alice after first game. Boils down to computing no of consecutive As and Bs anf the max wins.</t>
+  </si>
+  <si>
+    <t>subsets</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>Use backtrack. Empty arraylist. Add elements to it. Bactrack and then remove elements from it once all possibilities from that starting point are exhausted. Since empty set is a valid subset, make sure to add the empty arrayLst as well.</t>
+  </si>
+  <si>
+    <t>subsets without dups</t>
+  </si>
+  <si>
+    <t>permutations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use backtrack. Start with an empty arrayLsit and once its populated with all the elements(I.e len =  len of nums), then add it to final array. </t>
+  </si>
+  <si>
+    <t>permutations without dups</t>
+  </si>
+  <si>
+    <t>Same as perm 1. Only diff is sort the array and maintian a used array. If this value has been used or the previous occurance of current value hasn't been used yet, then don't use this value, use it only after previous usage, otherwis, will repeat permutaitons.</t>
+  </si>
+  <si>
+    <t>combination sum</t>
+  </si>
+  <si>
+    <t>Same as subsets, only difference is if the remainder value is 0, then add to final list, else don’t</t>
+  </si>
+  <si>
+    <t>combination sum without dups</t>
+  </si>
+  <si>
+    <t>Same as subsets 2 with the condition used as combo sum</t>
+  </si>
+  <si>
+    <t>Same as subsets, for duplicate, for index greater than start idx, if char is same as previous, don’t do anything. Make sure to sort</t>
+  </si>
+  <si>
+    <t>palindrome partitioning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use backtrack. Start with an empty arrayList, if there is a palindrome between start to I, then add it to the list. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time complexity: </t>
+  </si>
+  <si>
+    <t>O(N* 2^N)</t>
+  </si>
+  <si>
+    <t>Space complexity:</t>
+  </si>
+  <si>
+    <t>O(N)</t>
   </si>
 </sst>
 </file>
@@ -641,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0866E2BF-3754-D641-8414-7160098522DA}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1007,4 +1065,128 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA991216-2735-BF46-AEA3-CF251D7FD7ED}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="5"/>
+    <col min="3" max="3" width="141.6640625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>